<commit_message>
Aircraft functionality added, and the import of the importFlights added.
</commit_message>
<xml_diff>
--- a/Flights.xlsx
+++ b/Flights.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP-G4\IdeaProjects\unit3-project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\IdeaProjects\Projects\unit3-project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5F67CF-6CA0-4C11-8F16-228223EA06E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>nave31</t>
   </si>
@@ -114,12 +115,51 @@
   </si>
   <si>
     <t>23:00</t>
+  </si>
+  <si>
+    <t>Avianca</t>
+  </si>
+  <si>
+    <t>6/10/21</t>
+  </si>
+  <si>
+    <t>Taca</t>
+  </si>
+  <si>
+    <t>6/12/21</t>
+  </si>
+  <si>
+    <t>7:00</t>
+  </si>
+  <si>
+    <t>19:00</t>
+  </si>
+  <si>
+    <t>United</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>RF52</t>
+  </si>
+  <si>
+    <t>San Salvador</t>
+  </si>
+  <si>
+    <t>Lima, Peru</t>
+  </si>
+  <si>
+    <t>14/06/2021</t>
+  </si>
+  <si>
+    <t>5:50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -448,23 +488,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A6" sqref="A6:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -490,7 +530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -516,7 +556,7 @@
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -542,9 +582,9 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3.0</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
@@ -568,9 +608,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4.0</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -592,6 +632,136 @@
       </c>
       <c r="H5" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
export flight to pdf and excel
</commit_message>
<xml_diff>
--- a/Flights.xlsx
+++ b/Flights.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\IdeaProjects\Projects\unit3-project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP-G4\IdeaProjects\unit3-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5F67CF-6CA0-4C11-8F16-228223EA06E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>nave31</t>
   </si>
@@ -115,52 +114,12 @@
   </si>
   <si>
     <t>23:00</t>
-  </si>
-  <si>
-    <t>Avianca</t>
-  </si>
-  <si>
-    <t>6/10/21</t>
-  </si>
-  <si>
-    <t>Taca</t>
-  </si>
-  <si>
-    <t>6/12/21</t>
-  </si>
-  <si>
-    <t>7:00</t>
-  </si>
-  <si>
-    <t>19:00</t>
-  </si>
-  <si>
-    <t>United</t>
-  </si>
-  <si>
-    <t>Delta</t>
-  </si>
-  <si>
-    <t>RF52</t>
-  </si>
-  <si>
-    <t>San Salvador</t>
-  </si>
-  <si>
-    <t>Lima, Peru</t>
-  </si>
-  <si>
-    <t>14/06/2021</t>
-  </si>
-  <si>
-    <t>5:50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -488,23 +447,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -530,7 +489,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -556,7 +515,7 @@
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -582,7 +541,7 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -608,7 +567,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -632,136 +591,6 @@
       </c>
       <c r="H5" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>